<commit_message>
Fixed failing rspec tests
</commit_message>
<xml_diff>
--- a/spec/support/judgeNotInDb.xlsx
+++ b/spec/support/judgeNotInDb.xlsx
@@ -1,35 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE72DE7-2D8D-E542-85C2-9FE803ED4B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="18000" yWindow="1580" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId4"/>
+    <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
-  <si>
-    <t>Judge Non-Availability Dates</t>
-  </si>
-  <si>
-    <t>Judge Name</t>
-  </si>
-  <si>
-    <t>VLJ #</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Jones, Bernard</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>123</t>
   </si>
@@ -39,54 +30,55 @@
   <si>
     <t>456</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Scheduled For</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Regional Office</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>VLJ ID</t>
+  </si>
+  <si>
+    <t>VLJ</t>
+  </si>
+  <si>
+    <t>Hearings Scheduled</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>2 (1W200B)</t>
+  </si>
+  <si>
+    <t>1 of 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="13"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,24 +87,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="8"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -121,26 +101,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="10"/>
@@ -165,19 +125,6 @@
       </top>
       <bottom style="thin">
         <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -188,49 +135,12 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -278,15 +188,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -295,91 +196,6 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -398,128 +214,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,27 +238,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff595959"/>
-      <rgbColor rgb="ffdaeef3"/>
-      <rgbColor rgb="ff7f7f7f"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF595959"/>
+      <rgbColor rgb="FFDAEEF3"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -674,7 +442,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -683,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -692,7 +460,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -766,7 +534,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -774,7 +542,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -793,7 +561,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,7 +591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +721,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +747,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1044,9 +812,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1061,7 +835,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1069,7 +843,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1088,7 +862,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +888,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +914,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +940,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +966,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1218,7 +992,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,7 +1018,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1044,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1070,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1096,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1335,9 +1109,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1351,7 +1131,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1370,7 +1150,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1180,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1206,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1232,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1258,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,7 +1284,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1530,7 +1310,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1556,7 +1336,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1582,7 +1362,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1608,7 +1388,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1621,204 +1401,200 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8672" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5781" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8672" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8672" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="256" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47.1" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>43204</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2"/>
     </row>
-    <row r="2" ht="32.25" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" t="s" s="8">
+    <row r="3" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>43205</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s" s="10">
-        <v>3</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="6"/>
+      <c r="H3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
-    <row r="3" ht="35.1" customHeight="1">
-      <c r="A3" t="s" s="13">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s" s="14">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s" s="15">
-        <v>6</v>
-      </c>
-      <c r="D3" s="16">
-        <v>43467</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="6"/>
+    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" t="s" s="20">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="21">
-        <v>6</v>
-      </c>
-      <c r="D4" s="22">
-        <v>43498</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" t="s" s="20">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s" s="21">
-        <v>6</v>
-      </c>
-      <c r="D5" s="22">
-        <v>43498</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" t="s" s="20">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="21">
-        <v>6</v>
-      </c>
-      <c r="D6" s="22">
-        <v>43526</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="24"/>
-      <c r="B7" t="s" s="25">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>6</v>
-      </c>
-      <c r="D7" s="27">
-        <v>43557</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" t="s" s="29">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="30">
-        <v>6</v>
-      </c>
-      <c r="D8" s="31">
-        <v>43204</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+    <row r="9" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="32"/>
-      <c r="B9" t="s" s="33">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="34">
-        <v>8</v>
-      </c>
-      <c r="D9" s="35">
-        <v>43205</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
+    <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
update test spreadsheet & related tests
</commit_message>
<xml_diff>
--- a/spec/support/judgeNotInDb.xlsx
+++ b/spec/support/judgeNotInDb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navaloaner_2/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81E457E-13A0-FC4D-9D10-B14201A93837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D2BDD6-8C63-DF47-8FF9-8D01FE20097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15260" yWindow="1200" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Huels, Stuart</t>
-  </si>
-  <si>
-    <t>456</t>
   </si>
   <si>
     <t>ID</t>
@@ -55,13 +52,13 @@
     <t>2 (1W200B)</t>
   </si>
   <si>
-    <t>1 of 10</t>
-  </si>
-  <si>
     <t>CSS ID</t>
   </si>
   <si>
     <t>BVAHUELS</t>
+  </si>
+  <si>
+    <t>BVALAMPHERE</t>
   </si>
 </sst>
 </file>
@@ -71,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -81,6 +78,12 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -98,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,114 +110,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -222,21 +128,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1430,174 +1330,175 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>43204</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2"/>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="5">
         <v>43205</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Start work on better judge name validation
</commit_message>
<xml_diff>
--- a/spec/support/judgeNotInDb.xlsx
+++ b/spec/support/judgeNotInDb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navaloaner_2/workspace/caseflow/spec/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charley/Documents/programming/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D2BDD6-8C63-DF47-8FF9-8D01FE20097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A35FF4-02AB-6649-BBD5-16DE4C1FF7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Judge Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Huels, Stuart</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t>BVALAMPHERE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greneven, Eliana </t>
+  </si>
+  <si>
+    <t>BVAGRENEV</t>
+  </si>
+  <si>
+    <t>BVAMULLIGAN</t>
+  </si>
+  <si>
+    <t>Mulligan, James</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Virtual</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1348,7 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1423,48 +1441,104 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+    <row r="4" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43205</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+    <row r="5" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43205</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+    <row r="6" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>43205</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+    <row r="7" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>43205</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add tests and data for expected behavior
</commit_message>
<xml_diff>
--- a/spec/support/judgeNotInDb.xlsx
+++ b/spec/support/judgeNotInDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charley/Documents/programming/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A35FF4-02AB-6649-BBD5-16DE4C1FF7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A2C4A4-9B82-3E4B-908F-C2BB41D58276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Huels, Stuart</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Virtual</t>
+  </si>
+  <si>
+    <t>Morrigan, Jamess</t>
+  </si>
+  <si>
+    <t>BVAMORRIGA</t>
+  </si>
+  <si>
+    <t>BVANULLIGAM</t>
   </si>
 </sst>
 </file>
@@ -146,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -155,6 +164,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1348,7 +1358,7 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1359,7 +1369,7 @@
     <col min="4" max="4" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="256" width="11" style="1" customWidth="1"/>
   </cols>
@@ -1446,7 +1456,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>43205</v>
+        <v>43208</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1471,7 +1481,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>43205</v>
+        <v>43212</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -1496,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>43205</v>
+        <v>43213</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -1506,10 +1516,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -1521,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5">
-        <v>43205</v>
+        <v>43215</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1543,13 +1553,23 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="8">
+        <v>43216</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>